<commit_message>
update rumah dinas report
</commit_message>
<xml_diff>
--- a/report/Custom Report - Asset Rumah Dinas.xlsx
+++ b/report/Custom Report - Asset Rumah Dinas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="RUMAH DINAS" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>NO</t>
   </si>
@@ -54,9 +54,6 @@
     <t>WILAYAH</t>
   </si>
   <si>
-    <t>SATUAN</t>
-  </si>
-  <si>
     <t>NILAI BUKU</t>
   </si>
   <si>
@@ -91,6 +88,15 @@
   </si>
   <si>
     <t>${table:pk.NILAI_PERAWATAN}</t>
+  </si>
+  <si>
+    <t>STATUS KEPEMILIKAN</t>
+  </si>
+  <si>
+    <t>KETERANGAN</t>
+  </si>
+  <si>
+    <t>${table:pk.KETERANGAN}</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -209,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,31 +499,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
+    <col min="2" max="2" width="21.36328125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.44140625" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.08984375" customWidth="1"/>
+    <col min="11" max="11" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" customWidth="1"/>
+    <col min="20" max="20" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -534,25 +544,28 @@
         <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -566,36 +579,39 @@
         <v>7</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>